<commit_message>
prompts moved to files
</commit_message>
<xml_diff>
--- a/data/Questions/Fovea questions new.xlsx
+++ b/data/Questions/Fovea questions new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noesyssoft-my.sharepoint.com/personal/zeenat_noesyssoftware_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noesyssoft-my.sharepoint.com/personal/gautam_noesyssoftware_com/Documents/Documents/Projects/Infoverve-Helper/data/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2823" documentId="8_{F02AA5B8-29BE-4C43-BE0C-4A7244B62F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{018628A8-935A-4A6D-B911-7D1683649F1A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="696" yWindow="696" windowWidth="7500" windowHeight="6000" firstSheet="1" activeTab="3" xr2:uid="{31FC2E97-2AE2-4BDA-A719-AEAA7A33EA65}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{31FC2E97-2AE2-4BDA-A719-AEAA7A33EA65}"/>
   </bookViews>
   <sheets>
     <sheet name="videos" sheetId="1" r:id="rId1"/>
@@ -4081,8 +4081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221FEB25-AF78-4D99-913B-D9C9B2506117}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4321,7 +4321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0344418A-AD56-4554-910C-EF79D1A2CAAF}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -5148,6 +5148,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="aefbda5a-baf9-4cea-bcc4-fec604eaef94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100717F31954678894C858CE4F683EC3775" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21d292d56f77049c1169b58b57e3ac09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aefbda5a-baf9-4cea-bcc4-fec604eaef94" xmlns:ns4="8b9e4ac8-ea48-4416-81e6-df9438744b05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b43d6be8a8ada3f1ced01326eb0398d0" ns3:_="" ns4:_="">
     <xsd:import namespace="aefbda5a-baf9-4cea-bcc4-fec604eaef94"/>
@@ -5374,14 +5382,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="aefbda5a-baf9-4cea-bcc4-fec604eaef94" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DF3457B-C12E-49B3-AE8D-C1E543EDA2C6}">
   <ds:schemaRefs>
@@ -5391,6 +5391,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB27B031-DB7F-4B3B-8DC1-08EE35B17181}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8b9e4ac8-ea48-4416-81e6-df9438744b05"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="aefbda5a-baf9-4cea-bcc4-fec604eaef94"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{094461C6-8A85-4878-887C-DBF942583F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5407,21 +5424,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB27B031-DB7F-4B3B-8DC1-08EE35B17181}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8b9e4ac8-ea48-4416-81e6-df9438744b05"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="aefbda5a-baf9-4cea-bcc4-fec604eaef94"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
For each query part llm runs
</commit_message>
<xml_diff>
--- a/data/Questions/Fovea questions new.xlsx
+++ b/data/Questions/Fovea questions new.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2823" documentId="8_{F02AA5B8-29BE-4C43-BE0C-4A7244B62F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{018628A8-935A-4A6D-B911-7D1683649F1A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{31FC2E97-2AE2-4BDA-A719-AEAA7A33EA65}"/>
+    <workbookView minimized="1" xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{31FC2E97-2AE2-4BDA-A719-AEAA7A33EA65}"/>
   </bookViews>
   <sheets>
     <sheet name="videos" sheetId="1" r:id="rId1"/>
@@ -4081,8 +4081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221FEB25-AF78-4D99-913B-D9C9B2506117}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5148,14 +5148,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="aefbda5a-baf9-4cea-bcc4-fec604eaef94" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100717F31954678894C858CE4F683EC3775" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21d292d56f77049c1169b58b57e3ac09">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aefbda5a-baf9-4cea-bcc4-fec604eaef94" xmlns:ns4="8b9e4ac8-ea48-4416-81e6-df9438744b05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b43d6be8a8ada3f1ced01326eb0398d0" ns3:_="" ns4:_="">
     <xsd:import namespace="aefbda5a-baf9-4cea-bcc4-fec604eaef94"/>
@@ -5382,6 +5374,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="aefbda5a-baf9-4cea-bcc4-fec604eaef94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DF3457B-C12E-49B3-AE8D-C1E543EDA2C6}">
   <ds:schemaRefs>
@@ -5391,23 +5391,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB27B031-DB7F-4B3B-8DC1-08EE35B17181}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8b9e4ac8-ea48-4416-81e6-df9438744b05"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="aefbda5a-baf9-4cea-bcc4-fec604eaef94"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{094461C6-8A85-4878-887C-DBF942583F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5424,4 +5407,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB27B031-DB7F-4B3B-8DC1-08EE35B17181}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8b9e4ac8-ea48-4416-81e6-df9438744b05"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="aefbda5a-baf9-4cea-bcc4-fec604eaef94"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>